<commit_message>
kectura de excel bonita y pesos pueden ser None
</commit_message>
<xml_diff>
--- a/Harmonizer/datasets/matrix.xlsx
+++ b/Harmonizer/datasets/matrix.xlsx
@@ -441,27 +441,27 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>b3_-</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>4_-</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>b6_</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>b6_7</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>7_</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>b3_-</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>b6_7</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>b6_</t>
         </is>
       </c>
     </row>
@@ -475,10 +475,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
         <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -493,7 +493,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>4_-</t>
+          <t>b3_-</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -503,13 +503,13 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
         <v>1</v>
       </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -518,7 +518,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>7_</t>
+          <t>4_-</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -531,23 +531,23 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
         <v>1</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>b3_-</t>
+          <t>b6_</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -559,10 +559,10 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -575,13 +575,13 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -593,14 +593,14 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>b6_</t>
+          <t>7_</t>
         </is>
       </c>
       <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
         <v>1</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>

</xml_diff>